<commit_message>
modifikasi file excel untuk import pembayaran uas
</commit_message>
<xml_diff>
--- a/import/uas/pembayaran_uas.xlsx
+++ b/import/uas/pembayaran_uas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>2020/2021</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>tahun_ajaran (wajib diisi sesuai tahun ajaran saat ini)</t>
+  </si>
+  <si>
+    <t>Ani</t>
   </si>
 </sst>
 </file>
@@ -95,12 +98,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,12 +409,13 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.375" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
     <col min="6" max="6" width="43.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -441,16 +446,36 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="C2" s="3">
+        <v>44189</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44190</v>
+      </c>
+      <c r="D3">
+        <v>1000000</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>